<commit_message>
measure 2 by 2 similarity
</commit_message>
<xml_diff>
--- a/src/dataset/Questions.xlsx
+++ b/src/dataset/Questions.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,12 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Question</t>
   </si>
   <si>
-    <t xml:space="preserve">Why did Hitler attack the Soviet Union when he was still busy fighting the United Kingdom?</t>
+    <t xml:space="preserve">How can I chop onions without crying?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Why add salt to the water when cooking pasta?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How do you properly cook a steak?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How do you peel garlic easily?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How can I keep pasta from sticking to itself?</t>
   </si>
 </sst>
 </file>
@@ -40,6 +52,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -60,12 +73,14 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,13 +155,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="116.99"/>
   </cols>
@@ -159,6 +174,26 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>